<commit_message>
Added pkg repository/Added elections_1962
I added the basic package repository structure to the PolRD folder, under the name polDo. That is where all the package work will be done.

I also added the data for the 1962 elections and started working on it. So far I have changed the column names.
</commit_message>
<xml_diff>
--- a/tablas/formato_tablas.xlsx
+++ b/tablas/formato_tablas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\profesional\personal_projects\polRD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\profesional\personal_projects\polRD\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CD0331-E60E-463E-9794-0F7E6423EDC2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE58CFC6-CA17-451E-A0DD-9F643E12B9CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{4B4A90A2-7B00-4905-8F7F-B400F1541927}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>Ano</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t># inscritos</t>
+  </si>
+  <si>
+    <t>FP y aliados</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,7 +618,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -632,7 +635,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>2024</v>
+        <v>2020</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -647,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Tidied the dataset for 1962
There are some issues remaining:
Fix the encoding issue on 1962,
Save the dataset on the data folder,
Do the required documentation,
Change the values of the 'votos' variables to integers
</commit_message>
<xml_diff>
--- a/tablas/formato_tablas.xlsx
+++ b/tablas/formato_tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\profesional\personal_projects\polRD\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE58CFC6-CA17-451E-A0DD-9F643E12B9CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EC2AF2-F369-4FB9-9C42-D53102729A2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{4B4A90A2-7B00-4905-8F7F-B400F1541927}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>Ano</t>
   </si>
@@ -69,9 +69,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
     <t>Santiago</t>
   </si>
   <si>
@@ -109,6 +106,15 @@
   </si>
   <si>
     <t>FP y aliados</t>
+  </si>
+  <si>
+    <t>Observacion: aquellas columnas en amarillo definen una observacion atomica</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>DEPARTAMENTO</t>
   </si>
 </sst>
 </file>
@@ -468,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E123A7B-912B-4CD3-92A4-A5EB5D9A06C9}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,240 +490,236 @@
     <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2020</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
       </c>
       <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
-        <v>21</v>
+      <c r="M2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2020</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>11</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2020</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4">
         <v>1000</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2020</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
       <c r="H5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5">
         <v>700</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2024</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>9</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2024</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>9</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>